<commit_message>
Add tests for updateSpreadSheet. Add test spreadsheet.
#1 #2
</commit_message>
<xml_diff>
--- a/server/src/main/resources/IDPH_STD_Illinois_By_County_By_Sex.xlsx
+++ b/server/src/main/resources/IDPH_STD_Illinois_By_County_By_Sex.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="IDPH_STD_Illinois_By_County_By_Sex" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Early_Syphilis_Female_Count</t>
   </si>
   <si>
-    <t xml:space="preserve">Sort</t>
+    <t xml:space="preserve">#</t>
   </si>
   <si>
     <t xml:space="preserve">Cultivar</t>
@@ -382,6 +382,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -470,22 +471,22 @@
   <dimension ref="A1:J1668"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.04081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.6581632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>